<commit_message>
make all tests pass even with waits
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e19715a57ffb056d/Pulpit/Poważny tester/gyt/automation/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_AD4DADEC636C813AC809E43898996B645BDEDD8B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{068C44C9-F19C-4377-B968-B5344A63B817}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="11_AD4DADEC636C813AC809E43898996B645BDEDD8B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E65A9C56-FC2C-456E-A74C-81FD2255BED3}"/>
   <bookViews>
     <workbookView xWindow="3360" yWindow="885" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="signIn" sheetId="1" r:id="rId1"/>
-    <sheet name="offlineShopingProcess" sheetId="2" r:id="rId2"/>
+    <sheet name="offlineShopingProcess" sheetId="2" r:id="rId1"/>
+    <sheet name="signIn" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,35 +26,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>username</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>password</t>
   </si>
   <si>
-    <t>kacper@test</t>
-  </si>
-  <si>
     <t>haslo123</t>
   </si>
   <si>
-    <t>adam@test</t>
-  </si>
-  <si>
-    <t>123ABC</t>
-  </si>
-  <si>
-    <t>slym@test</t>
-  </si>
-  <si>
-    <t>bvcx</t>
-  </si>
-  <si>
-    <t>dżuls@testowa</t>
-  </si>
-  <si>
     <t>itemName</t>
   </si>
   <si>
@@ -95,6 +74,9 @@
   </si>
   <si>
     <t>Sopot</t>
+  </si>
+  <si>
+    <t>login</t>
   </si>
 </sst>
 </file>
@@ -426,71 +408,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>123456</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{AD5BB290-57A2-4D06-9C26-DBEE566A61DD}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{8CADB1C1-9540-42D9-BA05-013027A4BBE5}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{00CAF166-30F9-4D4F-83BC-7858698CE030}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{7BAE4192-39B4-4D6B-814A-2BCB69B3B3E8}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966F1E69-D2C9-4890-B8ED-8BBB93434CC5}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -501,48 +422,48 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <v>40600</v>
@@ -557,4 +478,38 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A449BB4-E1C0-49CE-88DB-5E9A2ADDF43C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{4E026729-202F-4A10-8924-2D8FD8DF4D6F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
remove all hardcoded test data
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e19715a57ffb056d/Pulpit/Poważny tester/gyt/automation/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="11_AD4DADEC636C813AC809E43898996B645BDEDD8B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E65A9C56-FC2C-456E-A74C-81FD2255BED3}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{77736C1D-2A92-4EF1-B33A-CA51484BDD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{316FFA12-2AF5-49B7-8477-51010DE87F0D}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="885" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3555" yWindow="5280" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="offlineShopingProcess" sheetId="2" r:id="rId1"/>
-    <sheet name="signIn" sheetId="3" r:id="rId2"/>
+    <sheet name="addToCartAndVerifyPrice" sheetId="4" r:id="rId2"/>
+    <sheet name="signIn" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>password</t>
   </si>
@@ -77,6 +78,27 @@
   </si>
   <si>
     <t>login</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>qnt</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -409,18 +431,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966F1E69-D2C9-4890-B8ED-8BBB93434CC5}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -440,13 +462,16 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -465,10 +490,13 @@
       <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2">
         <v>40600</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>123123123</v>
       </c>
     </row>
@@ -481,10 +509,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD142015-E182-4AE4-B907-D9A0CE10565A}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A449BB4-E1C0-49CE-88DB-5E9A2ADDF43C}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
cleaning add AddReviewTest class add new test to testng.xml
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e19715a57ffb056d/Pulpit/Poważny tester/gyt/automation/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{77736C1D-2A92-4EF1-B33A-CA51484BDD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{316FFA12-2AF5-49B7-8477-51010DE87F0D}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{77736C1D-2A92-4EF1-B33A-CA51484BDD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A16E6408-003D-419A-84C9-A149F648F70E}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="5280" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3210" yWindow="6990" windowWidth="21600" windowHeight="11325" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="offlineShopingProcess" sheetId="2" r:id="rId1"/>
     <sheet name="addToCartAndVerifyPrice" sheetId="4" r:id="rId2"/>
-    <sheet name="signIn" sheetId="3" r:id="rId3"/>
+    <sheet name="writeReview" sheetId="5" r:id="rId3"/>
+    <sheet name="signIn" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>password</t>
   </si>
@@ -99,6 +100,30 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>itemname</t>
+  </si>
+  <si>
+    <t>nick</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>Josie Yoga Jacket</t>
+  </si>
+  <si>
+    <t>janusz</t>
+  </si>
+  <si>
+    <t>niezła</t>
+  </si>
+  <si>
+    <t>niezła bluzka, taka niezbyt wygodna</t>
   </si>
 </sst>
 </file>
@@ -512,7 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD142015-E182-4AE4-B907-D9A0CE10565A}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -546,6 +571,50 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1101E95-46C0-423E-AD37-BE5729D19598}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A449BB4-E1C0-49CE-88DB-5E9A2ADDF43C}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
add driver to BasePage constructor some fun with Actions class
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e19715a57ffb056d/Pulpit/Poważny tester/gyt/automation/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{77736C1D-2A92-4EF1-B33A-CA51484BDD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A16E6408-003D-419A-84C9-A149F648F70E}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{77736C1D-2A92-4EF1-B33A-CA51484BDD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E73B8214-3EFE-4F79-9286-36180D8D6917}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="6990" windowWidth="21600" windowHeight="11325" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1785" yWindow="2310" windowWidth="21600" windowHeight="11325" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="offlineShopingProcess" sheetId="2" r:id="rId1"/>
     <sheet name="addToCartAndVerifyPrice" sheetId="4" r:id="rId2"/>
     <sheet name="writeReview" sheetId="5" r:id="rId3"/>
-    <sheet name="signIn" sheetId="3" r:id="rId4"/>
+    <sheet name="move" sheetId="6" r:id="rId4"/>
+    <sheet name="signIn" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>password</t>
   </si>
@@ -124,6 +125,9 @@
   </si>
   <si>
     <t>niezła bluzka, taka niezbyt wygodna</t>
+  </si>
+  <si>
+    <t>driver</t>
   </si>
 </sst>
 </file>
@@ -574,7 +578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1101E95-46C0-423E-AD37-BE5729D19598}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -615,6 +619,31 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F15B59-6BC2-43F4-82E0-07F044EA3290}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A449BB4-E1C0-49CE-88DB-5E9A2ADDF43C}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
upgrade xlxs with url data
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e19715a57ffb056d/Pulpit/Poważny tester/gyt/automation/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{77736C1D-2A92-4EF1-B33A-CA51484BDD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E73B8214-3EFE-4F79-9286-36180D8D6917}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{77736C1D-2A92-4EF1-B33A-CA51484BDD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{603958E4-4AB8-4AB3-B02B-2914258F1BC0}"/>
   <bookViews>
-    <workbookView xWindow="1785" yWindow="2310" windowWidth="21600" windowHeight="11325" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3915" yWindow="1440" windowWidth="21600" windowHeight="11325" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="offlineShopingProcess" sheetId="2" r:id="rId1"/>
     <sheet name="addToCartAndVerifyPrice" sheetId="4" r:id="rId2"/>
     <sheet name="writeReview" sheetId="5" r:id="rId3"/>
-    <sheet name="move" sheetId="6" r:id="rId4"/>
-    <sheet name="signIn" sheetId="3" r:id="rId5"/>
+    <sheet name="signIn" sheetId="3" r:id="rId4"/>
+    <sheet name="hoverToJackets" sheetId="7" r:id="rId5"/>
+    <sheet name="verifyLinking" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,14 +30,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>password</t>
   </si>
   <si>
-    <t>haslo123</t>
-  </si>
-  <si>
     <t>itemName</t>
   </si>
   <si>
@@ -127,14 +125,29 @@
     <t>niezła bluzka, taka niezbyt wygodna</t>
   </si>
   <si>
-    <t>driver</t>
+    <t>url</t>
+  </si>
+  <si>
+    <t>https://magento.softwaretestingboard.com/</t>
+  </si>
+  <si>
+    <t>https://magento.softwaretestingboard.com/customer/account/login/referer/</t>
+  </si>
+  <si>
+    <t>https://magento.softwaretestingboard.com/juno-jacket.html#</t>
+  </si>
+  <si>
+    <t>sistulostu@gufum.com</t>
+  </si>
+  <si>
+    <t>password!123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,6 +162,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -172,9 +191,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -460,112 +482,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966F1E69-D2C9-4890-B8ED-8BBB93434CC5}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2">
-        <v>40600</v>
-      </c>
-      <c r="I2">
-        <v>123123123</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{B2057B43-65C8-44B6-AE0B-ED97F66E342B}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD142015-E182-4AE4-B907-D9A0CE10565A}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2">
+        <v>40600</v>
+      </c>
+      <c r="J2">
+        <v>123123123</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{B2057B43-65C8-44B6-AE0B-ED97F66E342B}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD142015-E182-4AE4-B907-D9A0CE10565A}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2">
         <v>6</v>
       </c>
     </row>
@@ -576,40 +610,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1101E95-46C0-423E-AD37-BE5729D19598}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -619,60 +659,92 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F15B59-6BC2-43F4-82E0-07F044EA3290}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A449BB4-E1C0-49CE-88DB-5E9A2ADDF43C}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4E026729-202F-4A10-8924-2D8FD8DF4D6F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E7A97A-43C7-4D32-AB37-1519F5469B07}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C2502B-6BFB-4F78-99DD-1FAD25629DFC}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A449BB4-E1C0-49CE-88DB-5E9A2ADDF43C}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{4E026729-202F-4A10-8924-2D8FD8DF4D6F}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add WishListTest with data in xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e19715a57ffb056d/Pulpit/Poważny tester/gyt/automation/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{77736C1D-2A92-4EF1-B33A-CA51484BDD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{603958E4-4AB8-4AB3-B02B-2914258F1BC0}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{02FCFC9A-4B47-4B86-96D0-BBC7354EE355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89E80DBC-450A-47B0-9A51-B27EDD05B9D4}"/>
   <bookViews>
-    <workbookView xWindow="3915" yWindow="1440" windowWidth="21600" windowHeight="11325" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3915" yWindow="1440" windowWidth="21600" windowHeight="11325" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="offlineShopingProcess" sheetId="2" r:id="rId1"/>
     <sheet name="addToCartAndVerifyPrice" sheetId="4" r:id="rId2"/>
     <sheet name="writeReview" sheetId="5" r:id="rId3"/>
     <sheet name="signIn" sheetId="3" r:id="rId4"/>
-    <sheet name="hoverToJackets" sheetId="7" r:id="rId5"/>
-    <sheet name="verifyLinking" sheetId="8" r:id="rId6"/>
+    <sheet name="addToWishList" sheetId="9" r:id="rId5"/>
+    <sheet name="hoverToJackets" sheetId="7" r:id="rId6"/>
+    <sheet name="verifyLinking" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>password</t>
   </si>
@@ -191,10 +192,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -213,10 +217,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -662,6 +662,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A449BB4-E1C0-49CE-88DB-5E9A2ADDF43C}">
   <dimension ref="A1:C2"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4E026729-202F-4A10-8924-2D8FD8DF4D6F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E863D905-273D-4555-B2C6-C630230533B1}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
@@ -680,8 +720,8 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>33</v>
+      <c r="A2" t="s">
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>35</v>
@@ -692,13 +732,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{4E026729-202F-4A10-8924-2D8FD8DF4D6F}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{3CF250DF-9331-4DDD-A813-3007AFEFFD42}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34E7A97A-43C7-4D32-AB37-1519F5469B07}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -714,17 +755,20 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{0F7EE46D-33BB-419A-8985-82F643C4AE63}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C2502B-6BFB-4F78-99DD-1FAD25629DFC}">
   <dimension ref="A1:A2"/>
   <sheetViews>

</xml_diff>

<commit_message>
add change password test
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e19715a57ffb056d/Pulpit/Poważny tester/gyt/automation/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{02FCFC9A-4B47-4B86-96D0-BBC7354EE355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90BB5368-B40E-481B-B61B-A554BB87A98C}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{02FCFC9A-4B47-4B86-96D0-BBC7354EE355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8932AA04-A0F9-4F93-BB89-F6D04D31090A}"/>
   <bookViews>
-    <workbookView xWindow="3915" yWindow="1440" windowWidth="21600" windowHeight="11325" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="855" windowWidth="24885" windowHeight="12435" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="offlineShopingProcess" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,8 @@
     <sheet name="signIn" sheetId="3" r:id="rId4"/>
     <sheet name="addToWishList" sheetId="9" r:id="rId5"/>
     <sheet name="hoverToJackets" sheetId="7" r:id="rId6"/>
-    <sheet name="verifyLinking" sheetId="8" r:id="rId7"/>
+    <sheet name="changePassword" sheetId="12" r:id="rId7"/>
+    <sheet name="verifyLinking" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>password</t>
   </si>
@@ -142,6 +143,15 @@
   </si>
   <si>
     <t>password!123</t>
+  </si>
+  <si>
+    <t>listOption</t>
+  </si>
+  <si>
+    <t>currentPassword</t>
+  </si>
+  <si>
+    <t>newPassword</t>
   </si>
 </sst>
 </file>
@@ -667,7 +677,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -684,7 +694,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -697,6 +707,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{4E026729-202F-4A10-8924-2D8FD8DF4D6F}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{0A541EAE-0084-4EA5-A643-FFC2D300BC95}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -706,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E863D905-273D-4555-B2C6-C630230533B1}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -773,6 +784,64 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A530CA-21FA-4DE4-949A-87D204D8BD79}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{68CADBBD-1512-4473-BFC5-602858700BCB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C2502B-6BFB-4F78-99DD-1FAD25629DFC}">
   <dimension ref="A1:A2"/>
   <sheetViews>

</xml_diff>

<commit_message>
add add additional address test
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e19715a57ffb056d/Pulpit/Poważny tester/gyt/automation/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{02FCFC9A-4B47-4B86-96D0-BBC7354EE355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8932AA04-A0F9-4F93-BB89-F6D04D31090A}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{147675C9-8777-47A4-B2F3-ADB36E5AAAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6F83873-038C-44E3-9A1D-978113C161A4}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="855" windowWidth="24885" windowHeight="12435" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="885" windowWidth="24885" windowHeight="9195" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="offlineShopingProcess" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="addToWishList" sheetId="9" r:id="rId5"/>
     <sheet name="hoverToJackets" sheetId="7" r:id="rId6"/>
     <sheet name="changePassword" sheetId="12" r:id="rId7"/>
-    <sheet name="verifyLinking" sheetId="8" r:id="rId8"/>
+    <sheet name="addAdditionalAddress" sheetId="13" r:id="rId8"/>
+    <sheet name="verifyLinking" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>password</t>
   </si>
@@ -152,6 +153,30 @@
   </si>
   <si>
     <t>newPassword</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>11-222</t>
+  </si>
+  <si>
+    <t>poln 2</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>pomorskie</t>
+  </si>
+  <si>
+    <t>Poland</t>
   </si>
 </sst>
 </file>
@@ -227,10 +252,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -787,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0A530CA-21FA-4DE4-949A-87D204D8BD79}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -814,7 +835,7 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -836,12 +857,92 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{68CADBBD-1512-4473-BFC5-602858700BCB}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{8C37CCE1-0DCE-40DF-AA25-7E6FBC3ACA28}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92D7F04-DEA6-4802-BB22-AE6653F2BD83}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>123321</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C2502B-6BFB-4F78-99DD-1FAD25629DFC}">
   <dimension ref="A1:A2"/>
   <sheetViews>

</xml_diff>

<commit_message>
online shopping process test pt 1
</commit_message>
<xml_diff>
--- a/src/main/resources/testdata.xlsx
+++ b/src/main/resources/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e19715a57ffb056d/Pulpit/Poważny tester/gyt/automation/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{147675C9-8777-47A4-B2F3-ADB36E5AAAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E4FF353-3540-46E1-867F-D320F2A2F65D}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{C6B95B36-439F-4AA2-94FD-8FA3EB48F544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{089DFD30-C0CB-47E1-BEA6-D7DC643B62B3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="3630" windowWidth="20040" windowHeight="10200" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testOfflineShoppingProcess" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="testHoverToJackets" sheetId="7" r:id="rId6"/>
     <sheet name="testChangePassword" sheetId="12" r:id="rId7"/>
     <sheet name="testAddAddress" sheetId="13" r:id="rId8"/>
-    <sheet name="testNavMenuLinks" sheetId="8" r:id="rId9"/>
+    <sheet name="testOnlineShoppingProcess" sheetId="14" r:id="rId9"/>
+    <sheet name="testNavMenuLinks" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
   <si>
     <t>password</t>
   </si>
@@ -252,10 +253,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -604,6 +601,31 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C2502B-6BFB-4F78-99DD-1FAD25629DFC}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD142015-E182-4AE4-B907-D9A0CE10565A}">
   <dimension ref="A1:D2"/>
@@ -701,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A449BB4-E1C0-49CE-88DB-5E9A2ADDF43C}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -947,23 +969,35 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C2502B-6BFB-4F78-99DD-1FAD25629DFC}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D61B1C-B9AB-44F5-B454-18C74E4E69E3}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="2" t="s">
-        <v>32</v>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>